<commit_message>
M4 done - T_PS >=  3, without rankings
</commit_message>
<xml_diff>
--- a/Implementation/fyp_python/model3/M3_output_alloc_lteX.xlsx
+++ b/Implementation/fyp_python/model3/M3_output_alloc_lteX.xlsx
@@ -11424,7 +11424,7 @@
         <v>0</v>
       </c>
       <c r="BG21">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH21">
         <v>0</v>
@@ -12460,7 +12460,7 @@
         <v>0</v>
       </c>
       <c r="AO23">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP23">
         <v>0</v>
@@ -12571,7 +12571,7 @@
         <v>0</v>
       </c>
       <c r="BZ23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CA23">
         <v>0</v>
@@ -13556,7 +13556,7 @@
         <v>0</v>
       </c>
       <c r="AQ25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR25">
         <v>0</v>
@@ -13673,7 +13673,7 @@
         <v>0</v>
       </c>
       <c r="CD25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE25">
         <v>-0</v>
@@ -14068,7 +14068,7 @@
         <v>0</v>
       </c>
       <c r="AF26">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG26">
         <v>-0</v>
@@ -15251,7 +15251,7 @@
         <v>-0</v>
       </c>
       <c r="BK28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL28">
         <v>0</v>
@@ -19560,7 +19560,7 @@
         <v>0</v>
       </c>
       <c r="AT36">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AU36">
         <v>0</v>
@@ -21932,7 +21932,7 @@
         <v>1</v>
       </c>
       <c r="DF40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DG40">
         <v>0</v>
@@ -23360,7 +23360,7 @@
         <v>0</v>
       </c>
       <c r="AO43">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP43">
         <v>0</v>
@@ -24570,7 +24570,7 @@
         <v>0</v>
       </c>
       <c r="CC45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD45">
         <v>0</v>
@@ -24669,7 +24669,7 @@
         <v>0</v>
       </c>
       <c r="DJ45">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="DK45">
         <v>0</v>
@@ -31281,7 +31281,7 @@
         <v>0</v>
       </c>
       <c r="EH57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EI57">
         <v>0</v>
@@ -33284,7 +33284,7 @@
         <v>0</v>
       </c>
       <c r="CA61">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB61">
         <v>-0</v>
@@ -34383,7 +34383,7 @@
         <v>0</v>
       </c>
       <c r="CD63">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE63">
         <v>0</v>
@@ -35326,7 +35326,7 @@
         <v>0</v>
       </c>
       <c r="AG65">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AH65">
         <v>0</v>
@@ -35401,7 +35401,7 @@
         <v>0</v>
       </c>
       <c r="BF65">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BG65">
         <v>0</v>
@@ -35413,7 +35413,7 @@
         <v>0</v>
       </c>
       <c r="BJ65">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK65">
         <v>0</v>
@@ -35461,7 +35461,7 @@
         <v>0</v>
       </c>
       <c r="BZ65">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CA65">
         <v>0</v>
@@ -35686,7 +35686,7 @@
         <v>1</v>
       </c>
       <c r="EW65">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EX65">
         <v>0</v>
@@ -39114,7 +39114,7 @@
         <v>0</v>
       </c>
       <c r="X72">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Y72">
         <v>0</v>
@@ -40267,7 +40267,7 @@
         <v>0</v>
       </c>
       <c r="AS74">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AT74">
         <v>0</v>
@@ -42549,10 +42549,10 @@
         <v>0</v>
       </c>
       <c r="CA78">
+        <v>0</v>
+      </c>
+      <c r="CB78">
         <v>-0</v>
-      </c>
-      <c r="CB78">
-        <v>0</v>
       </c>
       <c r="CC78">
         <v>0</v>
@@ -43597,7 +43597,7 @@
         <v>0</v>
       </c>
       <c r="BM80">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BN80">
         <v>0</v>
@@ -44729,7 +44729,7 @@
         <v>0</v>
       </c>
       <c r="CA82">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB82">
         <v>0</v>
@@ -46304,7 +46304,7 @@
         <v>0</v>
       </c>
       <c r="BG85">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BH85">
         <v>0</v>
@@ -46583,7 +46583,7 @@
         <v>0</v>
       </c>
       <c r="EV85">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EW85">
         <v>0</v>
@@ -46819,7 +46819,7 @@
         <v>0</v>
       </c>
       <c r="AW86">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AX86">
         <v>0</v>
@@ -47358,7 +47358,7 @@
         <v>0</v>
       </c>
       <c r="AU87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV87">
         <v>0</v>
@@ -49098,7 +49098,7 @@
         <v>0</v>
       </c>
       <c r="CD90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE90">
         <v>0</v>
@@ -52263,7 +52263,7 @@
         <v>0</v>
       </c>
       <c r="AU96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV96">
         <v>0</v>
@@ -54961,7 +54961,7 @@
         <v>0</v>
       </c>
       <c r="AL101">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AM101">
         <v>0</v>
@@ -55812,7 +55812,7 @@
         <v>0</v>
       </c>
       <c r="EJ102">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EK102">
         <v>0</v>
@@ -56267,7 +56267,7 @@
         <v>-0</v>
       </c>
       <c r="DF103">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DG103">
         <v>0</v>
@@ -56725,7 +56725,7 @@
         <v>0</v>
       </c>
       <c r="CC104">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CD104">
         <v>0</v>
@@ -57749,7 +57749,7 @@
         <v>0</v>
       </c>
       <c r="BG106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BH106">
         <v>0</v>
@@ -59988,7 +59988,7 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:1">
@@ -60421,7 +60421,7 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -60496,7 +60496,7 @@
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:1">

</xml_diff>

<commit_message>
Model 2 working, Model 3 working
</commit_message>
<xml_diff>
--- a/Implementation/fyp_python/model3/M3_output_alloc_lteX.xlsx
+++ b/Implementation/fyp_python/model3/M3_output_alloc_lteX.xlsx
@@ -1,23 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwanakombohussein/Desktop/SPA_using_IP/Implementation/fyp_python/model3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EB84FC-9E10-0D4F-A165-6D1445C9ABEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="30420" windowHeight="20320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model3_alloc" sheetId="1" r:id="rId1"/>
     <sheet name="Model3_alloc_ranks" sheetId="2" r:id="rId2"/>
     <sheet name="Model3_alloc_lect_count" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,17 +64,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -100,7 +132,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -132,9 +164,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,6 +216,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -341,14 +409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FY109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:181">
+    <row r="1" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -893,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:181">
+    <row r="2" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1438,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:181">
+    <row r="3" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1983,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:181">
+    <row r="4" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2528,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:181">
+    <row r="5" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3073,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:181">
+    <row r="6" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3618,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:181">
+    <row r="7" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4163,7 +4231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:181">
+    <row r="8" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4708,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:181">
+    <row r="9" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5253,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:181">
+    <row r="10" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -5336,7 +5404,7 @@
         <v>1</v>
       </c>
       <c r="AB10">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -5798,7 +5866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:181">
+    <row r="11" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -5890,19 +5958,19 @@
         <v>0</v>
       </c>
       <c r="AE11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AH11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AJ11">
         <v>0</v>
@@ -6343,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:181">
+    <row r="12" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -6420,13 +6488,13 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <v>0</v>
       </c>
       <c r="AB12">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -6453,10 +6521,10 @@
         <v>1</v>
       </c>
       <c r="AK12">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AL12">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AM12">
         <v>0</v>
@@ -6888,7 +6956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:181">
+    <row r="13" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
@@ -6950,13 +7018,13 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V13">
         <v>0</v>
       </c>
       <c r="W13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -7007,19 +7075,19 @@
         <v>1</v>
       </c>
       <c r="AN13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AO13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AQ13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR13">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -7433,7 +7501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:181">
+    <row r="14" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
@@ -7510,7 +7578,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA14">
         <v>0</v>
@@ -7519,7 +7587,7 @@
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -7528,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="AF14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -7564,25 +7632,25 @@
         <v>0</v>
       </c>
       <c r="AR14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS14">
         <v>1</v>
       </c>
       <c r="AT14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AU14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AW14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AX14">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AY14">
         <v>0</v>
@@ -7978,7 +8046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:181">
+    <row r="15" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
@@ -8523,7 +8591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:181">
+    <row r="16" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
@@ -8651,10 +8719,10 @@
         <v>0</v>
       </c>
       <c r="AQ16">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR16">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -8696,10 +8764,10 @@
         <v>1</v>
       </c>
       <c r="BF16">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BG16">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH16">
         <v>0</v>
@@ -9068,7 +9136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:181">
+    <row r="17" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -9613,7 +9681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:181">
+    <row r="18" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -9714,7 +9782,7 @@
         <v>0</v>
       </c>
       <c r="AH18">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI18">
         <v>0</v>
@@ -9753,7 +9821,7 @@
         <v>0</v>
       </c>
       <c r="AU18">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV18">
         <v>0</v>
@@ -9801,7 +9869,7 @@
         <v>0</v>
       </c>
       <c r="BK18">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL18">
         <v>0</v>
@@ -10158,7 +10226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:181">
+    <row r="19" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -10235,7 +10303,7 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA19">
         <v>0</v>
@@ -10259,7 +10327,7 @@
         <v>0</v>
       </c>
       <c r="AH19">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI19">
         <v>0</v>
@@ -10703,7 +10771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:181">
+    <row r="20" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0</v>
       </c>
@@ -11248,7 +11316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:181">
+    <row r="21" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0</v>
       </c>
@@ -11337,7 +11405,7 @@
         <v>0</v>
       </c>
       <c r="AD21">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AE21">
         <v>0</v>
@@ -11793,7 +11861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:181">
+    <row r="22" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
@@ -12017,7 +12085,7 @@
         <v>0</v>
       </c>
       <c r="BW22">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BX22">
         <v>1</v>
@@ -12338,7 +12406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:181">
+    <row r="23" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0</v>
       </c>
@@ -12415,7 +12483,7 @@
         <v>0</v>
       </c>
       <c r="Z23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -12460,7 +12528,7 @@
         <v>0</v>
       </c>
       <c r="AO23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP23">
         <v>0</v>
@@ -12523,7 +12591,7 @@
         <v>0</v>
       </c>
       <c r="BJ23">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK23">
         <v>0</v>
@@ -12883,7 +12951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:181">
+    <row r="24" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0</v>
       </c>
@@ -12984,7 +13052,7 @@
         <v>0</v>
       </c>
       <c r="AH24">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI24">
         <v>0</v>
@@ -13119,13 +13187,13 @@
         <v>0</v>
       </c>
       <c r="CA24">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB24">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CC24">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CD24">
         <v>0</v>
@@ -13428,7 +13496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:181">
+    <row r="25" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0</v>
       </c>
@@ -13550,7 +13618,7 @@
         <v>0</v>
       </c>
       <c r="AO25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP25">
         <v>0</v>
@@ -13676,7 +13744,7 @@
         <v>0</v>
       </c>
       <c r="CE25">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CF25">
         <v>0</v>
@@ -13973,7 +14041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:181">
+    <row r="26" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0</v>
       </c>
@@ -14071,7 +14139,7 @@
         <v>0</v>
       </c>
       <c r="AG26">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AH26">
         <v>1</v>
@@ -14095,7 +14163,7 @@
         <v>0</v>
       </c>
       <c r="AO26">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP26">
         <v>0</v>
@@ -14104,7 +14172,7 @@
         <v>0</v>
       </c>
       <c r="AR26">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS26">
         <v>0</v>
@@ -14518,7 +14586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:181">
+    <row r="27" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
@@ -14595,13 +14663,13 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA27">
         <v>0</v>
       </c>
       <c r="AB27">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC27">
         <v>1</v>
@@ -14769,7 +14837,7 @@
         <v>0</v>
       </c>
       <c r="CF27">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CG27">
         <v>0</v>
@@ -15063,7 +15131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:181">
+    <row r="28" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0</v>
       </c>
@@ -15158,10 +15226,10 @@
         <v>0</v>
       </c>
       <c r="AF28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AH28">
         <v>0</v>
@@ -15209,7 +15277,7 @@
         <v>0</v>
       </c>
       <c r="AW28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AX28">
         <v>0</v>
@@ -15248,10 +15316,10 @@
         <v>0</v>
       </c>
       <c r="BJ28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL28">
         <v>0</v>
@@ -15296,7 +15364,7 @@
         <v>0</v>
       </c>
       <c r="BZ28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CA28">
         <v>0</v>
@@ -15320,7 +15388,7 @@
         <v>1</v>
       </c>
       <c r="CH28">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CI28">
         <v>0</v>
@@ -15608,7 +15676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:181">
+    <row r="29" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0</v>
       </c>
@@ -16153,7 +16221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:181">
+    <row r="30" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0</v>
       </c>
@@ -16248,7 +16316,7 @@
         <v>0</v>
       </c>
       <c r="AF30">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG30">
         <v>0</v>
@@ -16341,7 +16409,7 @@
         <v>0</v>
       </c>
       <c r="BK30">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL30">
         <v>0</v>
@@ -16407,7 +16475,7 @@
         <v>0</v>
       </c>
       <c r="CG30">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CH30">
         <v>0</v>
@@ -16698,7 +16766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:181">
+    <row r="31" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0</v>
       </c>
@@ -16802,7 +16870,7 @@
         <v>0</v>
       </c>
       <c r="AI31">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AJ31">
         <v>0</v>
@@ -16976,10 +17044,10 @@
         <v>1</v>
       </c>
       <c r="CO31">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CP31">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CQ31">
         <v>0</v>
@@ -17243,7 +17311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:181">
+    <row r="32" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0</v>
       </c>
@@ -17788,7 +17856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:181">
+    <row r="33" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0</v>
       </c>
@@ -18333,7 +18401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:181">
+    <row r="34" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0</v>
       </c>
@@ -18413,7 +18481,7 @@
         <v>0</v>
       </c>
       <c r="AA34">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AB34">
         <v>0</v>
@@ -18422,7 +18490,7 @@
         <v>0</v>
       </c>
       <c r="AD34">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AE34">
         <v>0</v>
@@ -18461,10 +18529,10 @@
         <v>0</v>
       </c>
       <c r="AQ34">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR34">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS34">
         <v>0</v>
@@ -18878,7 +18946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:181">
+    <row r="35" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -19423,7 +19491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:181">
+    <row r="36" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -19491,7 +19559,7 @@
         <v>0</v>
       </c>
       <c r="W36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X36">
         <v>0</v>
@@ -19500,13 +19568,13 @@
         <v>0</v>
       </c>
       <c r="Z36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA36">
         <v>0</v>
       </c>
       <c r="AB36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC36">
         <v>0</v>
@@ -19551,7 +19619,7 @@
         <v>0</v>
       </c>
       <c r="AQ36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR36">
         <v>0</v>
@@ -19560,7 +19628,7 @@
         <v>0</v>
       </c>
       <c r="AT36">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AU36">
         <v>0</v>
@@ -19968,7 +20036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:181">
+    <row r="37" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -20513,7 +20581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:181">
+    <row r="38" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -21058,7 +21126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:181">
+    <row r="39" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0</v>
       </c>
@@ -21159,7 +21227,7 @@
         <v>0</v>
       </c>
       <c r="AH39">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI39">
         <v>0</v>
@@ -21180,13 +21248,13 @@
         <v>0</v>
       </c>
       <c r="AO39">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP39">
         <v>0</v>
       </c>
       <c r="AQ39">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR39">
         <v>0</v>
@@ -21603,7 +21671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:181">
+    <row r="40" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -21686,7 +21754,7 @@
         <v>0</v>
       </c>
       <c r="AB40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC40">
         <v>0</v>
@@ -21704,7 +21772,7 @@
         <v>0</v>
       </c>
       <c r="AH40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI40">
         <v>0</v>
@@ -21743,7 +21811,7 @@
         <v>0</v>
       </c>
       <c r="AU40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV40">
         <v>0</v>
@@ -21791,7 +21859,7 @@
         <v>0</v>
       </c>
       <c r="BK40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL40">
         <v>0</v>
@@ -21800,7 +21868,7 @@
         <v>0</v>
       </c>
       <c r="BN40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO40">
         <v>0</v>
@@ -21932,7 +22000,7 @@
         <v>1</v>
       </c>
       <c r="DF40">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DG40">
         <v>0</v>
@@ -22148,7 +22216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:181">
+    <row r="41" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -22225,7 +22293,7 @@
         <v>0</v>
       </c>
       <c r="Z41">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA41">
         <v>0</v>
@@ -22249,7 +22317,7 @@
         <v>0</v>
       </c>
       <c r="AH41">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI41">
         <v>0</v>
@@ -22336,7 +22404,7 @@
         <v>0</v>
       </c>
       <c r="BK41">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL41">
         <v>0</v>
@@ -22474,7 +22542,7 @@
         <v>0</v>
       </c>
       <c r="DE41">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DF41">
         <v>0</v>
@@ -22693,7 +22761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:181">
+    <row r="42" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0</v>
       </c>
@@ -23010,23 +23078,23 @@
         <v>0</v>
       </c>
       <c r="DB42">
+        <v>0</v>
+      </c>
+      <c r="DC42">
+        <v>0</v>
+      </c>
+      <c r="DD42">
+        <v>0</v>
+      </c>
+      <c r="DE42">
+        <v>0</v>
+      </c>
+      <c r="DF42">
+        <v>0</v>
+      </c>
+      <c r="DG42">
         <v>1</v>
       </c>
-      <c r="DC42">
-        <v>0</v>
-      </c>
-      <c r="DD42">
-        <v>0</v>
-      </c>
-      <c r="DE42">
-        <v>0</v>
-      </c>
-      <c r="DF42">
-        <v>0</v>
-      </c>
-      <c r="DG42">
-        <v>0</v>
-      </c>
       <c r="DH42">
         <v>0</v>
       </c>
@@ -23238,7 +23306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:181">
+    <row r="43" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0</v>
       </c>
@@ -23306,7 +23374,7 @@
         <v>0</v>
       </c>
       <c r="W43">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X43">
         <v>0</v>
@@ -23315,13 +23383,13 @@
         <v>0</v>
       </c>
       <c r="Z43">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA43">
         <v>0</v>
       </c>
       <c r="AB43">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC43">
         <v>0</v>
@@ -23339,7 +23407,7 @@
         <v>0</v>
       </c>
       <c r="AH43">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI43">
         <v>0</v>
@@ -23360,7 +23428,7 @@
         <v>0</v>
       </c>
       <c r="AO43">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP43">
         <v>0</v>
@@ -23783,7 +23851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:181">
+    <row r="44" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0</v>
       </c>
@@ -23878,7 +23946,7 @@
         <v>0</v>
       </c>
       <c r="AF44">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG44">
         <v>0</v>
@@ -23968,7 +24036,7 @@
         <v>0</v>
       </c>
       <c r="BJ44">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK44">
         <v>0</v>
@@ -24016,7 +24084,7 @@
         <v>0</v>
       </c>
       <c r="BZ44">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CA44">
         <v>0</v>
@@ -24094,7 +24162,7 @@
         <v>0</v>
       </c>
       <c r="CZ44">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DA44">
         <v>0</v>
@@ -24328,7 +24396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:181">
+    <row r="45" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0</v>
       </c>
@@ -24399,7 +24467,7 @@
         <v>0</v>
       </c>
       <c r="X45">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Y45">
         <v>0</v>
@@ -24420,7 +24488,7 @@
         <v>0</v>
       </c>
       <c r="AE45">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF45">
         <v>0</v>
@@ -24588,7 +24656,7 @@
         <v>0</v>
       </c>
       <c r="CI45">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CJ45">
         <v>0</v>
@@ -24669,7 +24737,7 @@
         <v>0</v>
       </c>
       <c r="DJ45">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DK45">
         <v>0</v>
@@ -24873,7 +24941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:181">
+    <row r="46" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0</v>
       </c>
@@ -25217,7 +25285,7 @@
         <v>0</v>
       </c>
       <c r="DK46">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DL46">
         <v>0</v>
@@ -25418,7 +25486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:181">
+    <row r="47" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0</v>
       </c>
@@ -25489,7 +25557,7 @@
         <v>0</v>
       </c>
       <c r="X47">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Y47">
         <v>0</v>
@@ -25693,10 +25761,10 @@
         <v>0</v>
       </c>
       <c r="CN47">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CO47">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CP47">
         <v>1</v>
@@ -25768,10 +25836,10 @@
         <v>0</v>
       </c>
       <c r="DM47">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DN47">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DO47">
         <v>0</v>
@@ -25963,7 +26031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:181">
+    <row r="48" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0</v>
       </c>
@@ -26085,7 +26153,7 @@
         <v>0</v>
       </c>
       <c r="AO48">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP48">
         <v>0</v>
@@ -26160,7 +26228,7 @@
         <v>0</v>
       </c>
       <c r="BN48">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO48">
         <v>0</v>
@@ -26223,7 +26291,7 @@
         <v>0</v>
       </c>
       <c r="CI48">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CJ48">
         <v>0</v>
@@ -26319,7 +26387,7 @@
         <v>0</v>
       </c>
       <c r="DO48">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DP48">
         <v>0</v>
@@ -26508,7 +26576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:181">
+    <row r="49" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>0</v>
       </c>
@@ -26585,13 +26653,13 @@
         <v>0</v>
       </c>
       <c r="Z49">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA49">
         <v>0</v>
       </c>
       <c r="AB49">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC49">
         <v>0</v>
@@ -26609,7 +26677,7 @@
         <v>0</v>
       </c>
       <c r="AH49">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI49">
         <v>0</v>
@@ -26867,7 +26935,7 @@
         <v>0</v>
       </c>
       <c r="DP49">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DQ49">
         <v>0</v>
@@ -27053,7 +27121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:181">
+    <row r="50" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0</v>
       </c>
@@ -27598,7 +27666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:181">
+    <row r="51" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0</v>
       </c>
@@ -27774,7 +27842,7 @@
         <v>0</v>
       </c>
       <c r="BG51">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH51">
         <v>0</v>
@@ -28143,7 +28211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:181">
+    <row r="52" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>0</v>
       </c>
@@ -28397,7 +28465,7 @@
         <v>0</v>
       </c>
       <c r="CG52">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CH52">
         <v>0</v>
@@ -28523,10 +28591,10 @@
         <v>1</v>
       </c>
       <c r="DW52">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DX52">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DY52">
         <v>0</v>
@@ -28688,7 +28756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:181">
+    <row r="53" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>0</v>
       </c>
@@ -28780,10 +28848,10 @@
         <v>0</v>
       </c>
       <c r="AE53">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF53">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG53">
         <v>0</v>
@@ -29032,7 +29100,7 @@
         <v>0</v>
       </c>
       <c r="DK53">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DL53">
         <v>0</v>
@@ -29233,7 +29301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:181">
+    <row r="54" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0</v>
       </c>
@@ -29310,7 +29378,7 @@
         <v>0</v>
       </c>
       <c r="Z54">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA54">
         <v>0</v>
@@ -29778,7 +29846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:181">
+    <row r="55" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0</v>
       </c>
@@ -29963,7 +30031,7 @@
         <v>0</v>
       </c>
       <c r="BJ55">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK55">
         <v>0</v>
@@ -30011,7 +30079,7 @@
         <v>0</v>
       </c>
       <c r="BZ55">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CA55">
         <v>0</v>
@@ -30323,7 +30391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:181">
+    <row r="56" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>0</v>
       </c>
@@ -30403,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="AA56">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AB56">
         <v>0</v>
@@ -30415,7 +30483,7 @@
         <v>0</v>
       </c>
       <c r="AE56">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF56">
         <v>0</v>
@@ -30868,7 +30936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:181">
+    <row r="57" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>0</v>
       </c>
@@ -30963,7 +31031,7 @@
         <v>0</v>
       </c>
       <c r="AF57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG57">
         <v>0</v>
@@ -30993,13 +31061,13 @@
         <v>0</v>
       </c>
       <c r="AP57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AQ57">
         <v>0</v>
       </c>
       <c r="AR57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS57">
         <v>0</v>
@@ -31065,7 +31133,7 @@
         <v>0</v>
       </c>
       <c r="BN57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO57">
         <v>0</v>
@@ -31227,7 +31295,7 @@
         <v>0</v>
       </c>
       <c r="DP57">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DQ57">
         <v>0</v>
@@ -31413,7 +31481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:181">
+    <row r="58" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>0</v>
       </c>
@@ -31496,10 +31564,10 @@
         <v>0</v>
       </c>
       <c r="AB58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD58">
         <v>0</v>
@@ -31514,7 +31582,7 @@
         <v>0</v>
       </c>
       <c r="AH58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI58">
         <v>0</v>
@@ -31550,10 +31618,10 @@
         <v>0</v>
       </c>
       <c r="AT58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AU58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV58">
         <v>0</v>
@@ -31604,7 +31672,7 @@
         <v>0</v>
       </c>
       <c r="BL58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BM58">
         <v>0</v>
@@ -31658,7 +31726,7 @@
         <v>0</v>
       </c>
       <c r="CD58">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE58">
         <v>0</v>
@@ -31958,7 +32026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:181">
+    <row r="59" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>0</v>
       </c>
@@ -32503,7 +32571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:181">
+    <row r="60" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>0</v>
       </c>
@@ -32835,110 +32903,110 @@
         <v>0</v>
       </c>
       <c r="DG60">
+        <v>0</v>
+      </c>
+      <c r="DH60">
+        <v>0</v>
+      </c>
+      <c r="DI60">
+        <v>0</v>
+      </c>
+      <c r="DJ60">
+        <v>0</v>
+      </c>
+      <c r="DK60">
+        <v>0</v>
+      </c>
+      <c r="DL60">
+        <v>0</v>
+      </c>
+      <c r="DM60">
+        <v>0</v>
+      </c>
+      <c r="DN60">
+        <v>0</v>
+      </c>
+      <c r="DO60">
+        <v>0</v>
+      </c>
+      <c r="DP60">
+        <v>0</v>
+      </c>
+      <c r="DQ60">
+        <v>0</v>
+      </c>
+      <c r="DR60">
+        <v>0</v>
+      </c>
+      <c r="DS60">
+        <v>0</v>
+      </c>
+      <c r="DT60">
+        <v>0</v>
+      </c>
+      <c r="DU60">
+        <v>0</v>
+      </c>
+      <c r="DV60">
+        <v>0</v>
+      </c>
+      <c r="DW60">
+        <v>0</v>
+      </c>
+      <c r="DX60">
+        <v>0</v>
+      </c>
+      <c r="DY60">
+        <v>0</v>
+      </c>
+      <c r="DZ60">
+        <v>0</v>
+      </c>
+      <c r="EA60">
+        <v>0</v>
+      </c>
+      <c r="EB60">
+        <v>0</v>
+      </c>
+      <c r="EC60">
+        <v>0</v>
+      </c>
+      <c r="ED60">
+        <v>0</v>
+      </c>
+      <c r="EE60">
+        <v>0</v>
+      </c>
+      <c r="EF60">
+        <v>0</v>
+      </c>
+      <c r="EG60">
+        <v>0</v>
+      </c>
+      <c r="EH60">
+        <v>0</v>
+      </c>
+      <c r="EI60">
+        <v>0</v>
+      </c>
+      <c r="EJ60">
+        <v>0</v>
+      </c>
+      <c r="EK60">
+        <v>0</v>
+      </c>
+      <c r="EL60">
+        <v>0</v>
+      </c>
+      <c r="EM60">
+        <v>0</v>
+      </c>
+      <c r="EN60">
+        <v>0</v>
+      </c>
+      <c r="EO60">
         <v>1</v>
       </c>
-      <c r="DH60">
-        <v>0</v>
-      </c>
-      <c r="DI60">
-        <v>0</v>
-      </c>
-      <c r="DJ60">
-        <v>0</v>
-      </c>
-      <c r="DK60">
-        <v>0</v>
-      </c>
-      <c r="DL60">
-        <v>0</v>
-      </c>
-      <c r="DM60">
-        <v>0</v>
-      </c>
-      <c r="DN60">
-        <v>0</v>
-      </c>
-      <c r="DO60">
-        <v>0</v>
-      </c>
-      <c r="DP60">
-        <v>0</v>
-      </c>
-      <c r="DQ60">
-        <v>0</v>
-      </c>
-      <c r="DR60">
-        <v>0</v>
-      </c>
-      <c r="DS60">
-        <v>0</v>
-      </c>
-      <c r="DT60">
-        <v>0</v>
-      </c>
-      <c r="DU60">
-        <v>0</v>
-      </c>
-      <c r="DV60">
-        <v>0</v>
-      </c>
-      <c r="DW60">
-        <v>0</v>
-      </c>
-      <c r="DX60">
-        <v>0</v>
-      </c>
-      <c r="DY60">
-        <v>0</v>
-      </c>
-      <c r="DZ60">
-        <v>0</v>
-      </c>
-      <c r="EA60">
-        <v>0</v>
-      </c>
-      <c r="EB60">
-        <v>0</v>
-      </c>
-      <c r="EC60">
-        <v>0</v>
-      </c>
-      <c r="ED60">
-        <v>0</v>
-      </c>
-      <c r="EE60">
-        <v>0</v>
-      </c>
-      <c r="EF60">
-        <v>0</v>
-      </c>
-      <c r="EG60">
-        <v>0</v>
-      </c>
-      <c r="EH60">
-        <v>0</v>
-      </c>
-      <c r="EI60">
-        <v>0</v>
-      </c>
-      <c r="EJ60">
-        <v>0</v>
-      </c>
-      <c r="EK60">
-        <v>0</v>
-      </c>
-      <c r="EL60">
-        <v>0</v>
-      </c>
-      <c r="EM60">
-        <v>0</v>
-      </c>
-      <c r="EN60">
-        <v>0</v>
-      </c>
-      <c r="EO60">
-        <v>0</v>
-      </c>
       <c r="EP60">
         <v>0</v>
       </c>
@@ -33048,7 +33116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:181">
+    <row r="61" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>0</v>
       </c>
@@ -33125,7 +33193,7 @@
         <v>0</v>
       </c>
       <c r="Z61">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA61">
         <v>0</v>
@@ -33170,7 +33238,7 @@
         <v>0</v>
       </c>
       <c r="AO61">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP61">
         <v>0</v>
@@ -33287,13 +33355,13 @@
         <v>0</v>
       </c>
       <c r="CB61">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CC61">
         <v>0</v>
       </c>
       <c r="CD61">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE61">
         <v>0</v>
@@ -33488,7 +33556,7 @@
         <v>0</v>
       </c>
       <c r="EQ61">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="ER61">
         <v>0</v>
@@ -33593,7 +33661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:181">
+    <row r="62" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>0</v>
       </c>
@@ -34138,7 +34206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:181">
+    <row r="63" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>0</v>
       </c>
@@ -34215,13 +34283,13 @@
         <v>0</v>
       </c>
       <c r="Z63">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA63">
         <v>0</v>
       </c>
       <c r="AB63">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC63">
         <v>0</v>
@@ -34251,7 +34319,7 @@
         <v>0</v>
       </c>
       <c r="AL63">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AM63">
         <v>0</v>
@@ -34275,7 +34343,7 @@
         <v>0</v>
       </c>
       <c r="AT63">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AU63">
         <v>0</v>
@@ -34683,7 +34751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:181">
+    <row r="64" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>0</v>
       </c>
@@ -35228,7 +35296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:181">
+    <row r="65" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>0</v>
       </c>
@@ -35773,7 +35841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:181">
+    <row r="66" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>0</v>
       </c>
@@ -35841,7 +35909,7 @@
         <v>0</v>
       </c>
       <c r="W66">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X66">
         <v>0</v>
@@ -35850,7 +35918,7 @@
         <v>0</v>
       </c>
       <c r="Z66">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA66">
         <v>0</v>
@@ -35871,7 +35939,7 @@
         <v>0</v>
       </c>
       <c r="AG66">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AH66">
         <v>0</v>
@@ -36030,7 +36098,7 @@
         <v>0</v>
       </c>
       <c r="CH66">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CI66">
         <v>0</v>
@@ -36318,7 +36386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:181">
+    <row r="67" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>0</v>
       </c>
@@ -36395,13 +36463,13 @@
         <v>0</v>
       </c>
       <c r="Z67">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA67">
         <v>0</v>
       </c>
       <c r="AB67">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC67">
         <v>0</v>
@@ -36419,7 +36487,7 @@
         <v>0</v>
       </c>
       <c r="AH67">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI67">
         <v>0</v>
@@ -36863,7 +36931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:181">
+    <row r="68" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>0</v>
       </c>
@@ -37408,7 +37476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:181">
+    <row r="69" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>0</v>
       </c>
@@ -37494,7 +37562,7 @@
         <v>0</v>
       </c>
       <c r="AC69">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD69">
         <v>0</v>
@@ -37953,7 +38021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:181">
+    <row r="70" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>0</v>
       </c>
@@ -38033,7 +38101,7 @@
         <v>0</v>
       </c>
       <c r="AA70">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AB70">
         <v>0</v>
@@ -38045,7 +38113,7 @@
         <v>0</v>
       </c>
       <c r="AE70">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF70">
         <v>0</v>
@@ -38366,7 +38434,7 @@
         <v>0</v>
       </c>
       <c r="EH70">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EI70">
         <v>0</v>
@@ -38498,7 +38566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:181">
+    <row r="71" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>0</v>
       </c>
@@ -39043,7 +39111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:181">
+    <row r="72" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>0</v>
       </c>
@@ -39120,7 +39188,7 @@
         <v>0</v>
       </c>
       <c r="Z72">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA72">
         <v>0</v>
@@ -39150,7 +39218,7 @@
         <v>0</v>
       </c>
       <c r="AJ72">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AK72">
         <v>0</v>
@@ -39285,7 +39353,7 @@
         <v>0</v>
       </c>
       <c r="CC72">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CD72">
         <v>0</v>
@@ -39516,7 +39584,7 @@
         <v>0</v>
       </c>
       <c r="FB72">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FC72">
         <v>0</v>
@@ -39588,7 +39656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:181">
+    <row r="73" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>0</v>
       </c>
@@ -39674,7 +39742,7 @@
         <v>0</v>
       </c>
       <c r="AC73">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD73">
         <v>0</v>
@@ -39734,7 +39802,7 @@
         <v>0</v>
       </c>
       <c r="AW73">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AX73">
         <v>0</v>
@@ -40133,7 +40201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:181">
+    <row r="74" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>0</v>
       </c>
@@ -40210,16 +40278,16 @@
         <v>0</v>
       </c>
       <c r="Z74">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA74">
         <v>0</v>
       </c>
       <c r="AB74">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC74">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD74">
         <v>0</v>
@@ -40678,7 +40746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:181">
+    <row r="75" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>0</v>
       </c>
@@ -40758,7 +40826,7 @@
         <v>0</v>
       </c>
       <c r="AA75">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AB75">
         <v>0</v>
@@ -40770,10 +40838,10 @@
         <v>0</v>
       </c>
       <c r="AE75">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF75">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG75">
         <v>0</v>
@@ -41223,7 +41291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:181">
+    <row r="76" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>0</v>
       </c>
@@ -41384,7 +41452,7 @@
         <v>0</v>
       </c>
       <c r="BB76">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BC76">
         <v>0</v>
@@ -41453,7 +41521,7 @@
         <v>0</v>
       </c>
       <c r="BY76">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BZ76">
         <v>0</v>
@@ -41567,7 +41635,7 @@
         <v>0</v>
       </c>
       <c r="DK76">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DL76">
         <v>0</v>
@@ -41591,7 +41659,7 @@
         <v>0</v>
       </c>
       <c r="DS76">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DT76">
         <v>0</v>
@@ -41600,7 +41668,7 @@
         <v>0</v>
       </c>
       <c r="DV76">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DW76">
         <v>1</v>
@@ -41768,7 +41836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:181">
+    <row r="77" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>0</v>
       </c>
@@ -41866,10 +41934,10 @@
         <v>0</v>
       </c>
       <c r="AG77">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AH77">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI77">
         <v>0</v>
@@ -41908,7 +41976,7 @@
         <v>0</v>
       </c>
       <c r="AU77">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV77">
         <v>0</v>
@@ -42313,7 +42381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:181">
+    <row r="78" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>0</v>
       </c>
@@ -42381,7 +42449,7 @@
         <v>0</v>
       </c>
       <c r="W78">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X78">
         <v>0</v>
@@ -42435,7 +42503,7 @@
         <v>0</v>
       </c>
       <c r="AO78">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP78">
         <v>0</v>
@@ -42552,7 +42620,7 @@
         <v>0</v>
       </c>
       <c r="CB78">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CC78">
         <v>0</v>
@@ -42858,7 +42926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:181">
+    <row r="79" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>0</v>
       </c>
@@ -42986,7 +43054,7 @@
         <v>0</v>
       </c>
       <c r="AQ79">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR79">
         <v>1</v>
@@ -43055,7 +43123,7 @@
         <v>0</v>
       </c>
       <c r="BN79">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO79">
         <v>0</v>
@@ -43097,7 +43165,7 @@
         <v>0</v>
       </c>
       <c r="CB79">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CC79">
         <v>0</v>
@@ -43403,7 +43471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:181">
+    <row r="80" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>0</v>
       </c>
@@ -43486,7 +43554,7 @@
         <v>0</v>
       </c>
       <c r="AB80">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC80">
         <v>0</v>
@@ -43543,7 +43611,7 @@
         <v>0</v>
       </c>
       <c r="AU80">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV80">
         <v>0</v>
@@ -43597,7 +43665,7 @@
         <v>0</v>
       </c>
       <c r="BM80">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BN80">
         <v>0</v>
@@ -43897,7 +43965,7 @@
         <v>0</v>
       </c>
       <c r="FI80">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FJ80">
         <v>0</v>
@@ -43948,7 +44016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:181">
+    <row r="81" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>0</v>
       </c>
@@ -44493,7 +44561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:181">
+    <row r="82" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>0</v>
       </c>
@@ -44594,7 +44662,7 @@
         <v>0</v>
       </c>
       <c r="AH82">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI82">
         <v>0</v>
@@ -44729,7 +44797,7 @@
         <v>0</v>
       </c>
       <c r="CA82">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB82">
         <v>0</v>
@@ -45002,7 +45070,7 @@
         <v>0</v>
       </c>
       <c r="FN82">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FO82">
         <v>0</v>
@@ -45038,7 +45106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:181">
+    <row r="83" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>0</v>
       </c>
@@ -45223,7 +45291,7 @@
         <v>0</v>
       </c>
       <c r="BJ83">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK83">
         <v>0</v>
@@ -45583,7 +45651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:181">
+    <row r="84" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>0</v>
       </c>
@@ -45651,7 +45719,7 @@
         <v>0</v>
       </c>
       <c r="W84">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X84">
         <v>0</v>
@@ -45699,7 +45767,7 @@
         <v>0</v>
       </c>
       <c r="AM84">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AN84">
         <v>0</v>
@@ -45711,7 +45779,7 @@
         <v>0</v>
       </c>
       <c r="AQ84">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR84">
         <v>0</v>
@@ -46128,7 +46196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:181">
+    <row r="85" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>0</v>
       </c>
@@ -46214,7 +46282,7 @@
         <v>0</v>
       </c>
       <c r="AC85">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD85">
         <v>0</v>
@@ -46304,7 +46372,7 @@
         <v>0</v>
       </c>
       <c r="BG85">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH85">
         <v>0</v>
@@ -46673,7 +46741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:181">
+    <row r="86" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>0</v>
       </c>
@@ -46759,7 +46827,7 @@
         <v>0</v>
       </c>
       <c r="AC86">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD86">
         <v>0</v>
@@ -46768,7 +46836,7 @@
         <v>0</v>
       </c>
       <c r="AF86">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG86">
         <v>0</v>
@@ -46819,7 +46887,7 @@
         <v>0</v>
       </c>
       <c r="AW86">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AX86">
         <v>0</v>
@@ -46903,7 +46971,7 @@
         <v>0</v>
       </c>
       <c r="BY86">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BZ86">
         <v>0</v>
@@ -47185,7 +47253,7 @@
         <v>0</v>
       </c>
       <c r="FO86">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FP86">
         <v>0</v>
@@ -47218,7 +47286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:181">
+    <row r="87" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>0</v>
       </c>
@@ -47286,7 +47354,7 @@
         <v>0</v>
       </c>
       <c r="W87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X87">
         <v>0</v>
@@ -47310,7 +47378,7 @@
         <v>0</v>
       </c>
       <c r="AE87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF87">
         <v>0</v>
@@ -47328,7 +47396,7 @@
         <v>0</v>
       </c>
       <c r="AK87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AL87">
         <v>0</v>
@@ -47340,7 +47408,7 @@
         <v>0</v>
       </c>
       <c r="AO87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP87">
         <v>0</v>
@@ -47349,7 +47417,7 @@
         <v>0</v>
       </c>
       <c r="AR87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS87">
         <v>0</v>
@@ -47415,7 +47483,7 @@
         <v>0</v>
       </c>
       <c r="BN87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO87">
         <v>0</v>
@@ -47484,7 +47552,7 @@
         <v>0</v>
       </c>
       <c r="CK87">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CL87">
         <v>0</v>
@@ -47763,7 +47831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:181">
+    <row r="88" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>0</v>
       </c>
@@ -47999,7 +48067,7 @@
         <v>0</v>
       </c>
       <c r="CA88">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB88">
         <v>0</v>
@@ -48308,7 +48376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:181">
+    <row r="89" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>0</v>
       </c>
@@ -48391,7 +48459,7 @@
         <v>0</v>
       </c>
       <c r="AB89">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC89">
         <v>0</v>
@@ -48409,7 +48477,7 @@
         <v>0</v>
       </c>
       <c r="AH89">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI89">
         <v>0</v>
@@ -48436,7 +48504,7 @@
         <v>0</v>
       </c>
       <c r="AQ89">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR89">
         <v>0</v>
@@ -48451,7 +48519,7 @@
         <v>0</v>
       </c>
       <c r="AV89">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AW89">
         <v>0</v>
@@ -48853,7 +48921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:181">
+    <row r="90" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>0</v>
       </c>
@@ -48930,7 +48998,7 @@
         <v>0</v>
       </c>
       <c r="Z90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA90">
         <v>0</v>
@@ -48975,7 +49043,7 @@
         <v>0</v>
       </c>
       <c r="AO90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP90">
         <v>0</v>
@@ -48984,7 +49052,7 @@
         <v>0</v>
       </c>
       <c r="AR90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS90">
         <v>0</v>
@@ -49179,10 +49247,10 @@
         <v>0</v>
       </c>
       <c r="DE90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DF90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DG90">
         <v>0</v>
@@ -49293,7 +49361,7 @@
         <v>0</v>
       </c>
       <c r="EQ90">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="ER90">
         <v>0</v>
@@ -49398,7 +49466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:181">
+    <row r="91" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>0</v>
       </c>
@@ -49475,7 +49543,7 @@
         <v>0</v>
       </c>
       <c r="Z91">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA91">
         <v>0</v>
@@ -49655,7 +49723,7 @@
         <v>0</v>
       </c>
       <c r="CH91">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CI91">
         <v>0</v>
@@ -49664,7 +49732,7 @@
         <v>0</v>
       </c>
       <c r="CK91">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CL91">
         <v>0</v>
@@ -49943,7 +50011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:181">
+    <row r="92" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>0</v>
       </c>
@@ -50488,7 +50556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:181">
+    <row r="93" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>0</v>
       </c>
@@ -51033,7 +51101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:181">
+    <row r="94" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>0</v>
       </c>
@@ -51578,7 +51646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:181">
+    <row r="95" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>0</v>
       </c>
@@ -51640,7 +51708,7 @@
         <v>0</v>
       </c>
       <c r="U95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V95">
         <v>0</v>
@@ -51661,7 +51729,7 @@
         <v>0</v>
       </c>
       <c r="AB95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC95">
         <v>0</v>
@@ -51682,7 +51750,7 @@
         <v>0</v>
       </c>
       <c r="AI95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AJ95">
         <v>0</v>
@@ -51697,10 +51765,10 @@
         <v>0</v>
       </c>
       <c r="AN95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AO95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP95">
         <v>1</v>
@@ -51718,7 +51786,7 @@
         <v>0</v>
       </c>
       <c r="AU95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV95">
         <v>0</v>
@@ -51775,7 +51843,7 @@
         <v>0</v>
       </c>
       <c r="BN95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO95">
         <v>0</v>
@@ -51814,7 +51882,7 @@
         <v>0</v>
       </c>
       <c r="CA95">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB95">
         <v>0</v>
@@ -52123,7 +52191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:181">
+    <row r="96" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>0</v>
       </c>
@@ -52185,7 +52253,7 @@
         <v>0</v>
       </c>
       <c r="U96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V96">
         <v>0</v>
@@ -52206,7 +52274,7 @@
         <v>0</v>
       </c>
       <c r="AB96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC96">
         <v>0</v>
@@ -52245,7 +52313,7 @@
         <v>0</v>
       </c>
       <c r="AO96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AP96">
         <v>0</v>
@@ -52263,7 +52331,7 @@
         <v>0</v>
       </c>
       <c r="AU96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV96">
         <v>0</v>
@@ -52272,7 +52340,7 @@
         <v>0</v>
       </c>
       <c r="AX96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AY96">
         <v>0</v>
@@ -52359,10 +52427,10 @@
         <v>0</v>
       </c>
       <c r="CA96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CC96">
         <v>0</v>
@@ -52563,7 +52631,7 @@
         <v>0</v>
       </c>
       <c r="EQ96">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="ER96">
         <v>0</v>
@@ -52668,7 +52736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:181">
+    <row r="97" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>0</v>
       </c>
@@ -53213,7 +53281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:181">
+    <row r="98" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>0</v>
       </c>
@@ -53758,7 +53826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:181">
+    <row r="99" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>0</v>
       </c>
@@ -54303,7 +54371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:181">
+    <row r="100" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>0</v>
       </c>
@@ -54545,7 +54613,7 @@
         <v>0</v>
       </c>
       <c r="CC100">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CD100">
         <v>0</v>
@@ -54716,7 +54784,7 @@
         <v>0</v>
       </c>
       <c r="EH100">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EI100">
         <v>0</v>
@@ -54848,7 +54916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:181">
+    <row r="101" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>0</v>
       </c>
@@ -54961,7 +55029,7 @@
         <v>0</v>
       </c>
       <c r="AL101">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AM101">
         <v>0</v>
@@ -54988,7 +55056,7 @@
         <v>0</v>
       </c>
       <c r="AU101">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AV101">
         <v>0</v>
@@ -55072,7 +55140,7 @@
         <v>0</v>
       </c>
       <c r="BW101">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BX101">
         <v>0</v>
@@ -55102,7 +55170,7 @@
         <v>0</v>
       </c>
       <c r="CG101">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CH101">
         <v>0</v>
@@ -55393,7 +55461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:181">
+    <row r="102" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>0</v>
       </c>
@@ -55539,7 +55607,7 @@
         <v>0</v>
       </c>
       <c r="AW102">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AX102">
         <v>0</v>
@@ -55581,7 +55649,7 @@
         <v>0</v>
       </c>
       <c r="BK102">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL102">
         <v>0</v>
@@ -55647,7 +55715,7 @@
         <v>0</v>
       </c>
       <c r="CG102">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CH102">
         <v>0</v>
@@ -55938,7 +56006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:181">
+    <row r="103" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>0</v>
       </c>
@@ -56024,7 +56092,7 @@
         <v>0</v>
       </c>
       <c r="AC103">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AD103">
         <v>0</v>
@@ -56039,7 +56107,7 @@
         <v>0</v>
       </c>
       <c r="AH103">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI103">
         <v>0</v>
@@ -56264,7 +56332,7 @@
         <v>0</v>
       </c>
       <c r="DE103">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DF103">
         <v>0</v>
@@ -56483,7 +56551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:181">
+    <row r="104" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>0</v>
       </c>
@@ -56611,7 +56679,7 @@
         <v>0</v>
       </c>
       <c r="AQ104">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR104">
         <v>0</v>
@@ -56626,7 +56694,7 @@
         <v>0</v>
       </c>
       <c r="AV104">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AW104">
         <v>0</v>
@@ -57028,7 +57096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:181">
+    <row r="105" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>0</v>
       </c>
@@ -57129,7 +57197,7 @@
         <v>0</v>
       </c>
       <c r="AH105">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI105">
         <v>0</v>
@@ -57216,7 +57284,7 @@
         <v>0</v>
       </c>
       <c r="BK105">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL105">
         <v>0</v>
@@ -57537,7 +57605,7 @@
         <v>0</v>
       </c>
       <c r="FN105">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FO105">
         <v>0</v>
@@ -57573,7 +57641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:181">
+    <row r="106" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>0</v>
       </c>
@@ -57653,19 +57721,19 @@
         <v>0</v>
       </c>
       <c r="AA106">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AB106">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC106">
         <v>0</v>
       </c>
       <c r="AD106">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AE106">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF106">
         <v>0</v>
@@ -57749,7 +57817,7 @@
         <v>0</v>
       </c>
       <c r="BG106">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BH106">
         <v>0</v>
@@ -57914,7 +57982,7 @@
         <v>0</v>
       </c>
       <c r="DJ106">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DK106">
         <v>0</v>
@@ -58118,7 +58186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:181">
+    <row r="107" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>0</v>
       </c>
@@ -58354,7 +58422,7 @@
         <v>0</v>
       </c>
       <c r="CA107">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CB107">
         <v>0</v>
@@ -58663,7 +58731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:181">
+    <row r="108" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>0</v>
       </c>
@@ -58740,7 +58808,7 @@
         <v>0</v>
       </c>
       <c r="Z108">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA108">
         <v>0</v>
@@ -58908,7 +58976,7 @@
         <v>0</v>
       </c>
       <c r="CD108">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE108">
         <v>0</v>
@@ -58989,7 +59057,7 @@
         <v>0</v>
       </c>
       <c r="DE108">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DF108">
         <v>0</v>
@@ -59208,7 +59276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:181">
+    <row r="109" spans="1:181" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>0</v>
       </c>
@@ -59393,16 +59461,16 @@
         <v>0</v>
       </c>
       <c r="BJ109">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BK109">
         <v>0</v>
       </c>
       <c r="BL109">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BM109">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BN109">
         <v>0</v>
@@ -59465,7 +59533,7 @@
         <v>0</v>
       </c>
       <c r="CH109">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CI109">
         <v>0</v>
@@ -59759,554 +59827,554 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>3</v>
       </c>
@@ -60317,294 +60385,297 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="B1:I15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
+      <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>

</xml_diff>